<commit_message>
Some changes in few files.
</commit_message>
<xml_diff>
--- a/Git bash commands.xlsx
+++ b/Git bash commands.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\inASUS_TUF\Docs\Code\Git for me\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\inASUS_TUF\Docs\Code\Git_Local_Repositories\PersonalStuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BDBAC8-CE39-4188-8246-B0AC8835C39D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54346A4-C6C4-4BF5-BE73-17DDC2B45792}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" xr2:uid="{1DBC368A-6EAB-40F4-B912-9A25F29004D2}"/>
   </bookViews>
@@ -495,9 +495,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -505,6 +502,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -845,23 +845,23 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="4" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="E4" s="7" t="s">
+      <c r="C4" s="8"/>
+      <c r="E4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -974,10 +974,10 @@
       <c r="B16" s="2"/>
     </row>
     <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="7"/>
       <c r="E18" s="5" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Updating 'Git bash commands.xlsx', and adding 'Vim' folder for VIM configurations and commands inside the text editor.
</commit_message>
<xml_diff>
--- a/Git bash commands.xlsx
+++ b/Git bash commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\inASUS_TUF\Docs\Code\Git_Local_Repositories\PersonalStuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\1. PCs\1. inASUS_TUF\1. Documents\Code\Git for me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2C8EF5-B94E-4193-B878-01AB25422A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0889FE70-60C9-432B-AA13-2538232BE613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{1DBC368A-6EAB-40F4-B912-9A25F29004D2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1DBC368A-6EAB-40F4-B912-9A25F29004D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>Files</t>
   </si>
@@ -385,6 +385,18 @@
   </si>
   <si>
     <t>solve fatal: refusing to merge unrelated histories</t>
+  </si>
+  <si>
+    <t>show the differences between commits</t>
+  </si>
+  <si>
+    <t>git diff &lt;COMMIT&gt; &lt;ANOTHER_COMMIT&gt;</t>
+  </si>
+  <si>
+    <t>git checkout</t>
+  </si>
+  <si>
+    <t>show current branch</t>
   </si>
 </sst>
 </file>
@@ -480,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -495,7 +507,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -506,6 +518,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1158,11 +1173,11 @@
       <c r="C32" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>65</v>
+      <c r="E32" s="10" t="s">
+        <v>122</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1173,10 +1188,10 @@
         <v>104</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1186,11 +1201,11 @@
       <c r="C34" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>114</v>
+      <c r="E34" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1201,10 +1216,10 @@
         <v>108</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>70</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1214,11 +1229,11 @@
       <c r="C36" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>71</v>
+      <c r="E36" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>72</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1229,10 +1244,10 @@
         <v>109</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1243,10 +1258,10 @@
         <v>105</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1257,10 +1272,10 @@
         <v>106</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1271,10 +1286,10 @@
         <v>110</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1284,6 +1299,12 @@
       <c r="C41" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="E41" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="42" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="3" t="s">
@@ -1291,6 +1312,12 @@
       </c>
       <c r="C42" s="1" t="s">
         <v>111</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>